<commit_message>
Reworked conditional formatting behavior FIXED ~ Shifting Conditional Formats ~ Removing Conditional Formats ~ Copying Conditional Formats
ADDED

Conditional formats compress function
While saving, the conditional formats will be compressed
When cleaning a range, the conditional formatting will be removed
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Ranges/DeletingRanges.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Ranges/DeletingRanges.xlsx
@@ -398,9 +398,7 @@
     <x:col min="1" max="2" width="9.140625" style="2" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" s="2" customFormat="1">
-      <x:c r="A1" s="2" t="s"/>
-    </x:row>
+    <x:row r="1" spans="1:3" s="2" customFormat="1"/>
     <x:row r="2" spans="1:3" s="2" customFormat="1">
       <x:c r="B2" s="1" t="s"/>
       <x:c r="C2" s="1" t="s"/>

</xml_diff>

<commit_message>
Conditional formats shifting re-implemented. Reference file updated (empty cell excluded)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Ranges/DeletingRanges.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Ranges/DeletingRanges.xlsx
@@ -396,9 +396,7 @@
     <x:col min="1" max="2" width="9.140625" style="2" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" s="2" customFormat="1">
-      <x:c r="A1" s="2" t="s"/>
-    </x:row>
+    <x:row r="1" spans="1:3" s="2" customFormat="1"/>
     <x:row r="2" spans="1:3" s="2" customFormat="1">
       <x:c r="B2" s="1" t="s"/>
       <x:c r="C2" s="1" t="s"/>

</xml_diff>

<commit_message>
FIX Shifting conditional format ranges works slow and incorrectly (#721)
* Failing tests for conditional format shifting

* Conditional formats shifting re-implemented. Reference file updated (empty cell excluded)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Ranges/DeletingRanges.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Ranges/DeletingRanges.xlsx
@@ -396,9 +396,7 @@
     <x:col min="1" max="2" width="9.140625" style="2" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" s="2" customFormat="1">
-      <x:c r="A1" s="2" t="s"/>
-    </x:row>
+    <x:row r="1" spans="1:3" s="2" customFormat="1"/>
     <x:row r="2" spans="1:3" s="2" customFormat="1">
       <x:c r="B2" s="1" t="s"/>
       <x:c r="C2" s="1" t="s"/>

</xml_diff>

<commit_message>
Changed the cell ping behavior in the Row method to match the Column method Update reference files
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Ranges/DeletingRanges.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Ranges/DeletingRanges.xlsx
@@ -396,8 +396,12 @@
     <x:col min="1" max="2" width="9.140625" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" s="1" customFormat="1"/>
+    <x:row r="1" spans="1:3" s="1" customFormat="1">
+      <x:c r="A1" s="1" t="s"/>
+      <x:c r="B1" s="1" t="s"/>
+    </x:row>
     <x:row r="2" spans="1:3" s="1" customFormat="1">
+      <x:c r="A2" s="1" t="s"/>
       <x:c r="B2" s="2" t="s"/>
       <x:c r="C2" s="2" t="s"/>
     </x:row>

</xml_diff>